<commit_message>
Changement images par texte
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elmouctarsow/Desktop/Projet4ameliore/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B54E02-BA4D-E94A-9310-745DF464DF03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B6048D-7554-7744-8B69-EBCBFD4AA6DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25580" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>SEO</t>
   </si>
   <si>
-    <t>Le code source de chaque page contient une métadonnée qui en décrit le contenu</t>
-  </si>
-  <si>
     <t>Sans ces données, les outils de recherche extraient mal le contenu des pages</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
     <t xml:space="preserve">Rédiger un contenu permettant aux outils de recherche et d'améliorer les résultats de recherche. </t>
   </si>
   <si>
-    <t>Le titre de chaque page permet d'identifier le site</t>
-  </si>
-  <si>
     <t>Permettre aux utilisateurs d'identifier immédiatement le site dans les onglets, les favoris, dans la fenêtre du navigateur, ou encore dans les lecteurs d'écran,</t>
   </si>
   <si>
@@ -91,15 +85,9 @@
     <t>Donner un titre à l'ensemble des pages</t>
   </si>
   <si>
-    <t>Le titre de chaque page permet d'identifier son contenu.</t>
-  </si>
-  <si>
     <t>Meme éléments que celui d'en haut.</t>
   </si>
   <si>
-    <t xml:space="preserve">L'adresse complète et le numéro de téléphone des sociétés et organisations sont diponibles depuis toutes les pages du site. </t>
-  </si>
-  <si>
     <t>Donner aux utilisateurs qui le souhaitent la possibilité d'accéder sans difficulté aux moyens de contact téléphoniques et postaux</t>
   </si>
   <si>
@@ -109,9 +97,6 @@
     <t>Manque d'accessibilité du site sans une adresse complète</t>
   </si>
   <si>
-    <t>Chaque image décorative est dotée d'une alternative textuelle appropriée</t>
-  </si>
-  <si>
     <t>Fournir aux robots d'indexation uniquement des informations pertinentes</t>
   </si>
   <si>
@@ -124,9 +109,6 @@
     <t>Le non renseignement de cette alternative textuelle freine l'accessibilité du site</t>
   </si>
   <si>
-    <t>Le contenu de chaque page est organisé selon une structure de titres et sous-titres hiérarchisée.</t>
-  </si>
-  <si>
     <t>Permettre aux machines et aux outils d'indexation d'extraire le plan de chaque page</t>
   </si>
   <si>
@@ -139,9 +121,6 @@
     <t xml:space="preserve">Hiérarchiser les titres, de H1 on arrive à H2 ainsi de suite </t>
   </si>
   <si>
-    <t>Chaque lien est doté d'un intitulé dans le code source</t>
-  </si>
-  <si>
     <t>Éviter aux utilisateurs d'avoir uniquement une URL peu compréhensible en guise de libellé,</t>
   </si>
   <si>
@@ -157,9 +136,6 @@
     <t>Doté de chaque lien un intitulé dans le code source</t>
   </si>
   <si>
-    <t>Les liens sont visuellement différenciés du reste du contenu</t>
-  </si>
-  <si>
     <t>Améliorer la visibilité et l'affordance des liens</t>
   </si>
   <si>
@@ -184,9 +160,6 @@
     <t xml:space="preserve">Veuillez à ce que chaque page ait un seul identifiant </t>
   </si>
   <si>
-    <t>Optimisation des images</t>
-  </si>
-  <si>
     <t>Mettre sur le format Jpeg au lieu de Bmp</t>
   </si>
   <si>
@@ -229,9 +202,6 @@
     <t xml:space="preserve">Créer un fichier sitemap.xml contenant la liste des pages du site à la racine du site. À defaut de respecter le format XML, une simple liste d'URL est acceptée par les moteurs. </t>
   </si>
   <si>
-    <t xml:space="preserve">Les scripts du site sont minifiés </t>
-  </si>
-  <si>
     <t>Accélère la viteese d'affichage des pages</t>
   </si>
   <si>
@@ -250,9 +220,6 @@
     <t>ou identifier la liste des scripts Javascript non minifiés à l'aide d'outil de développement (navigateurs, outils en ligne, etc..)</t>
   </si>
   <si>
-    <t>Les feuilles de style du site sont minifiés</t>
-  </si>
-  <si>
     <t>Minimiser la quantité de données à télécharger par l'utilisateur</t>
   </si>
   <si>
@@ -280,7 +247,40 @@
     <t>Renseigner la balise robot à la page HTML index meta name="robot"</t>
   </si>
   <si>
-    <t>La racine du site contient des instructions pour les robots d'indexation</t>
+    <t>Le code source de la page principale (index) contient une métadonnée répétitive qui ne décrit pas son contenu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le titre de la page2 ne permet pas d'identifier le site, il doit être reformulé. </t>
+  </si>
+  <si>
+    <t>Le titre des pages ne permet pas d'identifier son contenu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'adresse complète n'existe pas pour toutes les pages du site, et le numéro de téléphone des sociétés et organisations n'existent pas. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les images décoratives ne sont pas dotées d'une alternative textuelle appropriée.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le contenu des pages ne respectent la hiérarchie selon une structure de titres et sous-titres. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La racine du site ne contient pas des instructions pour les robots d'indexation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les liens ne sont pas dotés d'un intitulé dans le code source. </t>
+  </si>
+  <si>
+    <t>Visuellement les liens ne sont pas différenciés du reste du contenu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les images ne sont pas optimisées, elles sont lourdes, avec une grande taille. Elles empêchent le site de se charger vite. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les feuilles de style du site sont à minifier, elles comportent beaucoup de lignes. Les navigateurs prennent du temps à les lire. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les scripts du site doivent être minifiées, ils comportent beacoup, de lignes, des commentaires. Ce qui ralenti le chargement des pages.  </t>
   </si>
 </sst>
 </file>
@@ -794,14 +794,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="52.140625" customWidth="1"/>
+    <col min="2" max="2" width="77.7109375" customWidth="1"/>
     <col min="3" max="5" width="45.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
     <col min="7" max="26" width="10.5703125" customWidth="1"/>
@@ -852,26 +852,26 @@
         <v>9</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14"/>
       <c r="B3" s="6"/>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -881,7 +881,7 @@
       <c r="A4" s="14"/>
       <c r="B4" s="6"/>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -890,26 +890,26 @@
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="6" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -919,7 +919,7 @@
       <c r="A7" s="14"/>
       <c r="B7" s="6"/>
       <c r="C7" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -929,7 +929,7 @@
       <c r="A8" s="14"/>
       <c r="B8" s="6"/>
       <c r="C8" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -938,40 +938,40 @@
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9" s="6" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="15" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23"/>
       <c r="B10" s="6" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="6"/>
       <c r="C11" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -980,26 +980,26 @@
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
       <c r="B12" s="6" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
       <c r="B13" s="6"/>
       <c r="C13" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="3"/>
@@ -1008,54 +1008,54 @@
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
       <c r="B14" s="6" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="15" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="24"/>
       <c r="B15" s="25"/>
       <c r="C15" s="26" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F15" s="27"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="9" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -1065,7 +1065,7 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1075,7 +1075,7 @@
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
@@ -1087,26 +1087,26 @@
         <v>7</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="3"/>
       <c r="C22" s="9" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1116,7 +1116,7 @@
       <c r="A23" s="14"/>
       <c r="B23" s="3"/>
       <c r="C23" s="9" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -1125,26 +1125,26 @@
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="6" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14"/>
       <c r="B25" s="3"/>
       <c r="C25" s="9" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1153,26 +1153,26 @@
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
       <c r="B26" s="6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
       <c r="B27" s="3"/>
       <c r="C27" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1182,7 +1182,7 @@
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
       <c r="C28" s="22" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="18"/>
@@ -1194,48 +1194,48 @@
         <v>8</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14"/>
       <c r="B31" s="6"/>
       <c r="C31" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1249,26 +1249,26 @@
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14"/>
       <c r="B34" s="6" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="6"/>
       <c r="C35" s="9" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1277,26 +1277,26 @@
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="14"/>
       <c r="B36" s="6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="14"/>
       <c r="B37" s="3"/>
       <c r="C37" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -1305,30 +1305,30 @@
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="14"/>
       <c r="B38" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="14"/>
       <c r="B39" s="3"/>
       <c r="C39" s="4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="4" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F39" s="15"/>
     </row>
@@ -1336,7 +1336,7 @@
       <c r="A40" s="14"/>
       <c r="B40" s="3"/>
       <c r="C40" s="4" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -1346,7 +1346,7 @@
       <c r="A41" s="17"/>
       <c r="B41" s="18"/>
       <c r="C41" s="19" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>

</xml_diff>